<commit_message>
Add convert Census Excel
</commit_message>
<xml_diff>
--- a/Medical__NBQ804.xlsx
+++ b/Medical__NBQ804.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\excel\Request_Med\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sudeepa.w\Documents\GitHub\AlgoSpring-ISON\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE8622E0-670D-4161-8797-06EBBD948004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A66997-16C4-4D56-9E5B-5B312D8585CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{C0FDBFCA-7D5A-476A-866F-82BE3E666118}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{C0FDBFCA-7D5A-476A-866F-82BE3E666118}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -720,9 +720,9 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -871,7 +871,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>79</v>
       </c>
@@ -1014,7 +1014,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>100</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>101</v>
       </c>
@@ -1311,9 +1311,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1321,7 +1325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1329,7 +1333,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1337,7 +1341,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1345,7 +1349,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1353,7 +1357,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1361,7 +1365,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1369,7 +1373,7 @@
         <v>971545079578</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1377,7 +1381,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1385,7 +1389,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1393,7 +1397,7 @@
         <v>45598</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1401,7 +1405,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1409,7 +1413,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -1417,7 +1421,7 @@
         <v>10345</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1425,12 +1429,12 @@
         <v>45598</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1438,7 +1442,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -1446,7 +1450,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -1454,7 +1458,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>

</xml_diff>